<commit_message>
Order of questions changed
</commit_message>
<xml_diff>
--- a/app/config/tables/VAC/forms/VAC_CRIANCA/VAC_CRIANCA.xlsx
+++ b/app/config/tables/VAC/forms/VAC_CRIANCA/VAC_CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE570BE-6087-474F-999C-75E347DF94C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCFD70B-760D-4F45-ADE4-9E0DD22B78C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1493,7 +1493,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1515,6 +1515,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -1918,9 +1921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:J250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38:F41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5093,7 +5096,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5602,7 +5605,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="12"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H19" s="12"/>
@@ -5921,7 +5924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B236" sqref="B236"/>
     </sheetView>

</xml_diff>